<commit_message>
Top 5 e ajustes matrizes derivadas
</commit_message>
<xml_diff>
--- a/Topicos Fundamentais/Top5/TRU/TRU_VA_corrente_2010.xlsx
+++ b/Topicos Fundamentais/Top5/TRU/TRU_VA_corrente_2010.xlsx
@@ -3,340 +3,343 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
-  <si>
-    <t>0191
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0191
 Agricultura, inclusive o apoio à agricultura e a pós-colheita</t>
   </si>
   <si>
-    <t>0192
+    <t xml:space="preserve">0192
 Pecuária, inclusive o apoio à pecuária</t>
   </si>
   <si>
-    <t>0280
+    <t xml:space="preserve">0280
 Produção florestal; pesca e aquicultura</t>
   </si>
   <si>
-    <t>0580
+    <t xml:space="preserve">0580
 Extração de carvão mineral e de minerais não-metálicos</t>
   </si>
   <si>
-    <t>0680
+    <t xml:space="preserve">0680
 Extração de petróleo e gás, inclusive as atividades de apoio</t>
   </si>
   <si>
-    <t>0791
+    <t xml:space="preserve">0791
 Extração de minério de ferro, inclusive beneficiamentos e a aglomeração</t>
   </si>
   <si>
-    <t>0792
+    <t xml:space="preserve">0792
 Extração de minerais metálicos não-ferrosos, inclusive beneficiamentos</t>
   </si>
   <si>
-    <t>1091
+    <t xml:space="preserve">1091
 Abate e produtos de carne, inclusive os produtos do laticínio e da pesca</t>
   </si>
   <si>
-    <t>1092
+    <t xml:space="preserve">1092
 Fabricação e refino de açúcar</t>
   </si>
   <si>
-    <t>1093
+    <t xml:space="preserve">1093
 Outros produtos alimentares</t>
   </si>
   <si>
-    <t>1100
+    <t xml:space="preserve">1100
 Fabricação de bebidas</t>
   </si>
   <si>
-    <t>1200
+    <t xml:space="preserve">1200
 Fabricação de produtos do fumo</t>
   </si>
   <si>
-    <t>1300
+    <t xml:space="preserve">1300
 Fabricação de produtos têxteis</t>
   </si>
   <si>
-    <t>1400
+    <t xml:space="preserve">1400
 Confecção de artefatos do vestuário e acessórios</t>
   </si>
   <si>
-    <t>1500
+    <t xml:space="preserve">1500
 Fabricação de calçados e de artefatos de couro</t>
   </si>
   <si>
-    <t>1600
+    <t xml:space="preserve">1600
 Fabricação de produtos da madeira</t>
   </si>
   <si>
-    <t>1700
+    <t xml:space="preserve">1700
 Fabricação de celulose, papel e produtos de papel</t>
   </si>
   <si>
-    <t>1800
+    <t xml:space="preserve">1800
 Impressão e reprodução de gravações</t>
   </si>
   <si>
-    <t>1991
+    <t xml:space="preserve">1991
 Refino de petróleo e coquerias</t>
   </si>
   <si>
-    <t>1992
+    <t xml:space="preserve">1992
 Fabricação de biocombustíveis</t>
   </si>
   <si>
-    <t>2091
+    <t xml:space="preserve">2091
 Fabricação de químicos orgânicos e inorgânicos, resinas e elastômeros</t>
   </si>
   <si>
-    <t>2092
+    <t xml:space="preserve">2092
 Fabricação de defensivos, desinfestantes, tintas e químicos diversos</t>
   </si>
   <si>
-    <t>2093
+    <t xml:space="preserve">2093
 Fabricação de produtos de limpeza, cosméticos/perfumaria e higiene pessoal</t>
   </si>
   <si>
-    <t>2100
+    <t xml:space="preserve">2100
 Fabricação de produtos farmoquímicos e farmacêuticos</t>
   </si>
   <si>
-    <t>2200
+    <t xml:space="preserve">2200
 Fabricação de produtos de borracha e de material plástico</t>
   </si>
   <si>
-    <t>2300
+    <t xml:space="preserve">2300
 Fabricação de produtos de minerais não-metálicos</t>
   </si>
   <si>
-    <t>2491
+    <t xml:space="preserve">2491
 Produção de ferro-gusa/ferroligas, siderurgia e tubos de aço sem costura</t>
   </si>
   <si>
-    <t>2492
+    <t xml:space="preserve">2492
 Metalurgia de metais não-ferrosos e a fundição de metais</t>
   </si>
   <si>
-    <t>2500
+    <t xml:space="preserve">2500
 Fabricação de produtos de metal, exceto máquinas e equipamentos</t>
   </si>
   <si>
-    <t>2600
+    <t xml:space="preserve">2600
 Fabricação de equipamentos de informática, produtos eletrônicos e ópticos</t>
   </si>
   <si>
-    <t>2700
+    <t xml:space="preserve">2700
 Fabricação de máquinas e equipamentos elétricos</t>
   </si>
   <si>
-    <t>2800
+    <t xml:space="preserve">2800
 Fabricação de máquinas e equipamentos mecânicos</t>
   </si>
   <si>
-    <t>2991
+    <t xml:space="preserve">2991
 Fabricação de automóveis, caminhões e ônibus, exceto peças</t>
   </si>
   <si>
-    <t>2992
+    <t xml:space="preserve">2992
 Fabricação de peças e acessórios para veículos automotores</t>
   </si>
   <si>
-    <t>3000
+    <t xml:space="preserve">3000
 Fabricação de outros equipamentos de transporte, exceto veículos automotores</t>
   </si>
   <si>
-    <t>3180
+    <t xml:space="preserve">3180
 Fabricação de móveis e de produtos de indústrias diversas</t>
   </si>
   <si>
-    <t>3300
+    <t xml:space="preserve">3300
 Manutenção, reparação e instalação de máquinas e equipamentos</t>
   </si>
   <si>
-    <t>3500
+    <t xml:space="preserve">3500
 Energia elétrica, gás natural e outras utilidades</t>
   </si>
   <si>
-    <t>3680
+    <t xml:space="preserve">3680
 Água, esgoto e gestão de resíduos</t>
   </si>
   <si>
-    <t>4180
+    <t xml:space="preserve">4180
 Construção</t>
   </si>
   <si>
-    <t>4500
+    <t xml:space="preserve">4500
 Comércio e reparação de veículos automotores e motocicletas</t>
   </si>
   <si>
-    <t>4680
+    <t xml:space="preserve">4680
 Comércio por atacado e a varejo, exceto veículos automotores</t>
   </si>
   <si>
-    <t>4900
+    <t xml:space="preserve">4900
 Transporte terrestre</t>
   </si>
   <si>
-    <t>5000
+    <t xml:space="preserve">5000
 Transporte aquaviário</t>
   </si>
   <si>
-    <t>5100
+    <t xml:space="preserve">5100
 Transporte aéreo</t>
   </si>
   <si>
-    <t>5280
+    <t xml:space="preserve">5280
 Armazenamento, atividades auxiliares dos transportes e correio</t>
   </si>
   <si>
-    <t>5500
+    <t xml:space="preserve">5500
 Alojamento</t>
   </si>
   <si>
-    <t>5600
+    <t xml:space="preserve">5600
 Alimentação</t>
   </si>
   <si>
-    <t>5800
+    <t xml:space="preserve">5800
 Edição e edição integrada à impressão</t>
   </si>
   <si>
-    <t>5980
+    <t xml:space="preserve">5980
 Atividades de televisão, rádio, cinema e  gravação/edição de som e imagem</t>
   </si>
   <si>
-    <t>6100
+    <t xml:space="preserve">6100
 Telecomunicações</t>
   </si>
   <si>
-    <t>6280
+    <t xml:space="preserve">6280
 Desenvolvimento de sistemas e outros serviços de informação</t>
   </si>
   <si>
-    <t>6480
+    <t xml:space="preserve">6480
 Intermediação financeira, seguros e previdência complementar</t>
   </si>
   <si>
-    <t>6800
+    <t xml:space="preserve">6800
 Atividades imobiliárias</t>
   </si>
   <si>
-    <t>6980
+    <t xml:space="preserve">6980
 Atividades jurídicas, contábeis, consultoria e sedes de empresas</t>
   </si>
   <si>
-    <t>7180
+    <t xml:space="preserve">7180
 Serviços de arquitetura, engenharia, testes/análises técnicas e P &amp; D</t>
   </si>
   <si>
-    <t>7380
+    <t xml:space="preserve">7380
 Outras atividades profissionais, científicas e técnicas</t>
   </si>
   <si>
-    <t>7700
+    <t xml:space="preserve">7700
 Aluguéis não-imobiliários e gestão de ativos de propriedade intelectual</t>
   </si>
   <si>
-    <t>7880
+    <t xml:space="preserve">7880
 Outras atividades administrativas e serviços complementares</t>
   </si>
   <si>
-    <t>8000
+    <t xml:space="preserve">8000
 Atividades de vigilância, segurança e investigação</t>
   </si>
   <si>
-    <t>8400
+    <t xml:space="preserve">8400
 Administração pública, defesa e seguridade social</t>
   </si>
   <si>
-    <t>8591
+    <t xml:space="preserve">8591
 Educação pública</t>
   </si>
   <si>
-    <t>8592
+    <t xml:space="preserve">8592
 Educação privada</t>
   </si>
   <si>
-    <t>8691
+    <t xml:space="preserve">8691
 Saúde pública</t>
   </si>
   <si>
-    <t>8692
+    <t xml:space="preserve">8692
 Saúde privada</t>
   </si>
   <si>
-    <t>9080
+    <t xml:space="preserve">9080
 Atividades artísticas, criativas e de espetáculos</t>
   </si>
   <si>
-    <t>9480
+    <t xml:space="preserve">9480
 Organizações associativas e outros serviços pessoais</t>
   </si>
   <si>
-    <t>9700
+    <t xml:space="preserve">9700
 Serviços domésticos</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t xml:space="preserve">Valor adicionado bruto ( PIB )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remunerações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salários</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contribuições sociais efetivas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previdência oficial /FGTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previdência privada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contribuições sociais imputadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excedente operacional bruto e rendimento misto bruto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rendimento misto bruto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excedente operacional bruto (EOB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outros impostos sobre a produção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outros subsídios à produção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor da produção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fator trabalho (ocupações)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11.0"/>
-      <color indexed="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -347,7 +350,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -365,3151 +368,3435 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AG1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AH1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AK1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AL1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AM1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AN1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AP1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AQ1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AR1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AS1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AT1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AU1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AV1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AW1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AX1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AY1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AZ1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BA1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BC1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BD1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BE1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BF1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="BG1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BH1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BI1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BK1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BL1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="BM1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BN1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BO1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BP1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BQ1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" t="n">
-        <v>100111.0</v>
+        <v>100111</v>
       </c>
       <c r="C2" t="n">
-        <v>44863.0</v>
+        <v>44863</v>
       </c>
       <c r="D2" t="n">
-        <v>14958.0</v>
+        <v>14958</v>
       </c>
       <c r="E2" t="n">
-        <v>6592.0</v>
+        <v>6592</v>
       </c>
       <c r="F2" t="n">
-        <v>63474.0</v>
+        <v>63474</v>
       </c>
       <c r="G2" t="n">
-        <v>36491.0</v>
+        <v>36491</v>
       </c>
       <c r="H2" t="n">
-        <v>3408.0</v>
+        <v>3408</v>
       </c>
       <c r="I2" t="n">
-        <v>20849.0</v>
+        <v>20849</v>
       </c>
       <c r="J2" t="n">
-        <v>9545.0</v>
+        <v>9545</v>
       </c>
       <c r="K2" t="n">
-        <v>27485.0</v>
+        <v>27485</v>
       </c>
       <c r="L2" t="n">
-        <v>17224.0</v>
+        <v>17224</v>
       </c>
       <c r="M2" t="n">
-        <v>3595.0</v>
+        <v>3595</v>
       </c>
       <c r="N2" t="n">
-        <v>10950.0</v>
+        <v>10950</v>
       </c>
       <c r="O2" t="n">
-        <v>22027.0</v>
+        <v>22027</v>
       </c>
       <c r="P2" t="n">
-        <v>10553.0</v>
+        <v>10553</v>
       </c>
       <c r="Q2" t="n">
-        <v>8536.0</v>
+        <v>8536</v>
       </c>
       <c r="R2" t="n">
-        <v>15334.0</v>
+        <v>15334</v>
       </c>
       <c r="S2" t="n">
-        <v>7518.0</v>
+        <v>7518</v>
       </c>
       <c r="T2" t="n">
-        <v>16329.0</v>
+        <v>16329</v>
       </c>
       <c r="U2" t="n">
-        <v>5370.0</v>
+        <v>5370</v>
       </c>
       <c r="V2" t="n">
-        <v>14430.0</v>
+        <v>14430</v>
       </c>
       <c r="W2" t="n">
-        <v>9028.0</v>
+        <v>9028</v>
       </c>
       <c r="X2" t="n">
-        <v>7136.0</v>
+        <v>7136</v>
       </c>
       <c r="Y2" t="n">
-        <v>19526.0</v>
+        <v>19526</v>
       </c>
       <c r="Z2" t="n">
-        <v>21322.0</v>
+        <v>21322</v>
       </c>
       <c r="AA2" t="n">
-        <v>22348.0</v>
+        <v>22348</v>
       </c>
       <c r="AB2" t="n">
-        <v>16931.0</v>
+        <v>16931</v>
       </c>
       <c r="AC2" t="n">
-        <v>7269.0</v>
+        <v>7269</v>
       </c>
       <c r="AD2" t="n">
-        <v>29401.0</v>
+        <v>29401</v>
       </c>
       <c r="AE2" t="n">
-        <v>13958.0</v>
+        <v>13958</v>
       </c>
       <c r="AF2" t="n">
-        <v>14641.0</v>
+        <v>14641</v>
       </c>
       <c r="AG2" t="n">
-        <v>30905.0</v>
+        <v>30905</v>
       </c>
       <c r="AH2" t="n">
-        <v>38191.0</v>
+        <v>38191</v>
       </c>
       <c r="AI2" t="n">
-        <v>23875.0</v>
+        <v>23875</v>
       </c>
       <c r="AJ2" t="n">
-        <v>9449.0</v>
+        <v>9449</v>
       </c>
       <c r="AK2" t="n">
-        <v>23502.0</v>
+        <v>23502</v>
       </c>
       <c r="AL2" t="n">
-        <v>17125.0</v>
+        <v>17125</v>
       </c>
       <c r="AM2" t="n">
-        <v>68868.0</v>
+        <v>68868</v>
       </c>
       <c r="AN2" t="n">
-        <v>24046.0</v>
+        <v>24046</v>
       </c>
       <c r="AO2" t="n">
-        <v>206927.0</v>
+        <v>206927</v>
       </c>
       <c r="AP2" t="n">
-        <v>65757.0</v>
+        <v>65757</v>
       </c>
       <c r="AQ2" t="n">
-        <v>350472.0</v>
+        <v>350472</v>
       </c>
       <c r="AR2" t="n">
-        <v>93150.0</v>
+        <v>93150</v>
       </c>
       <c r="AS2" t="n">
-        <v>3505.0</v>
+        <v>3505</v>
       </c>
       <c r="AT2" t="n">
-        <v>6257.0</v>
+        <v>6257</v>
       </c>
       <c r="AU2" t="n">
-        <v>38748.0</v>
+        <v>38748</v>
       </c>
       <c r="AV2" t="n">
-        <v>8519.0</v>
+        <v>8519</v>
       </c>
       <c r="AW2" t="n">
-        <v>61685.0</v>
+        <v>61685</v>
       </c>
       <c r="AX2" t="n">
-        <v>10549.0</v>
+        <v>10549</v>
       </c>
       <c r="AY2" t="n">
-        <v>12302.0</v>
+        <v>12302</v>
       </c>
       <c r="AZ2" t="n">
-        <v>58171.0</v>
+        <v>58171</v>
       </c>
       <c r="BA2" t="n">
-        <v>45520.0</v>
+        <v>45520</v>
       </c>
       <c r="BB2" t="n">
-        <v>224561.0</v>
+        <v>224561</v>
       </c>
       <c r="BC2" t="n">
-        <v>274420.0</v>
+        <v>274420</v>
       </c>
       <c r="BD2" t="n">
-        <v>77760.0</v>
+        <v>77760</v>
       </c>
       <c r="BE2" t="n">
-        <v>30003.0</v>
+        <v>30003</v>
       </c>
       <c r="BF2" t="n">
-        <v>19285.0</v>
+        <v>19285</v>
       </c>
       <c r="BG2" t="n">
-        <v>16106.0</v>
+        <v>16106</v>
       </c>
       <c r="BH2" t="n">
-        <v>85574.0</v>
+        <v>85574</v>
       </c>
       <c r="BI2" t="n">
-        <v>16990.0</v>
+        <v>16990</v>
       </c>
       <c r="BJ2" t="n">
-        <v>343319.0</v>
+        <v>343319</v>
       </c>
       <c r="BK2" t="n">
-        <v>127157.0</v>
+        <v>127157</v>
       </c>
       <c r="BL2" t="n">
-        <v>36830.0</v>
+        <v>36830</v>
       </c>
       <c r="BM2" t="n">
-        <v>67369.0</v>
+        <v>67369</v>
       </c>
       <c r="BN2" t="n">
-        <v>62184.0</v>
+        <v>62184</v>
       </c>
       <c r="BO2" t="n">
-        <v>14312.0</v>
+        <v>14312</v>
       </c>
       <c r="BP2" t="n">
-        <v>47911.0</v>
+        <v>47911</v>
       </c>
       <c r="BQ2" t="n">
-        <v>40334.0</v>
+        <v>40334</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3" t="n">
-        <v>21587.0</v>
+        <v>21587</v>
       </c>
       <c r="C3" t="n">
-        <v>14062.0</v>
+        <v>14062</v>
       </c>
       <c r="D3" t="n">
-        <v>1983.0</v>
+        <v>1983</v>
       </c>
       <c r="E3" t="n">
-        <v>2772.0</v>
+        <v>2772</v>
       </c>
       <c r="F3" t="n">
-        <v>12201.0</v>
+        <v>12201</v>
       </c>
       <c r="G3" t="n">
-        <v>3687.0</v>
+        <v>3687</v>
       </c>
       <c r="H3" t="n">
-        <v>1507.0</v>
+        <v>1507</v>
       </c>
       <c r="I3" t="n">
-        <v>13111.0</v>
+        <v>13111</v>
       </c>
       <c r="J3" t="n">
-        <v>6175.0</v>
+        <v>6175</v>
       </c>
       <c r="K3" t="n">
-        <v>16095.0</v>
+        <v>16095</v>
       </c>
       <c r="L3" t="n">
-        <v>5267.0</v>
+        <v>5267</v>
       </c>
       <c r="M3" t="n">
-        <v>1148.0</v>
+        <v>1148</v>
       </c>
       <c r="N3" t="n">
-        <v>8058.0</v>
+        <v>8058</v>
       </c>
       <c r="O3" t="n">
-        <v>12199.0</v>
+        <v>12199</v>
       </c>
       <c r="P3" t="n">
-        <v>7847.0</v>
+        <v>7847</v>
       </c>
       <c r="Q3" t="n">
-        <v>4658.0</v>
+        <v>4658</v>
       </c>
       <c r="R3" t="n">
-        <v>7965.0</v>
+        <v>7965</v>
       </c>
       <c r="S3" t="n">
-        <v>4217.0</v>
+        <v>4217</v>
       </c>
       <c r="T3" t="n">
-        <v>4075.0</v>
+        <v>4075</v>
       </c>
       <c r="U3" t="n">
-        <v>2609.0</v>
+        <v>2609</v>
       </c>
       <c r="V3" t="n">
-        <v>6738.0</v>
+        <v>6738</v>
       </c>
       <c r="W3" t="n">
-        <v>5842.0</v>
+        <v>5842</v>
       </c>
       <c r="X3" t="n">
-        <v>3568.0</v>
+        <v>3568</v>
       </c>
       <c r="Y3" t="n">
-        <v>6320.0</v>
+        <v>6320</v>
       </c>
       <c r="Z3" t="n">
-        <v>13312.0</v>
+        <v>13312</v>
       </c>
       <c r="AA3" t="n">
-        <v>11954.0</v>
+        <v>11954</v>
       </c>
       <c r="AB3" t="n">
-        <v>8817.0</v>
+        <v>8817</v>
       </c>
       <c r="AC3" t="n">
-        <v>4579.0</v>
+        <v>4579</v>
       </c>
       <c r="AD3" t="n">
-        <v>16938.0</v>
+        <v>16938</v>
       </c>
       <c r="AE3" t="n">
-        <v>8232.0</v>
+        <v>8232</v>
       </c>
       <c r="AF3" t="n">
-        <v>10457.0</v>
+        <v>10457</v>
       </c>
       <c r="AG3" t="n">
-        <v>18897.0</v>
+        <v>18897</v>
       </c>
       <c r="AH3" t="n">
-        <v>14987.0</v>
+        <v>14987</v>
       </c>
       <c r="AI3" t="n">
-        <v>15509.0</v>
+        <v>15509</v>
       </c>
       <c r="AJ3" t="n">
-        <v>6121.0</v>
+        <v>6121</v>
       </c>
       <c r="AK3" t="n">
-        <v>9652.0</v>
+        <v>9652</v>
       </c>
       <c r="AL3" t="n">
-        <v>7491.0</v>
+        <v>7491</v>
       </c>
       <c r="AM3" t="n">
-        <v>12131.0</v>
+        <v>12131</v>
       </c>
       <c r="AN3" t="n">
-        <v>8106.0</v>
+        <v>8106</v>
       </c>
       <c r="AO3" t="n">
-        <v>81713.0</v>
+        <v>81713</v>
       </c>
       <c r="AP3" t="n">
-        <v>28094.0</v>
+        <v>28094</v>
       </c>
       <c r="AQ3" t="n">
-        <v>162106.0</v>
+        <v>162106</v>
       </c>
       <c r="AR3" t="n">
-        <v>43846.0</v>
+        <v>43846</v>
       </c>
       <c r="AS3" t="n">
-        <v>2414.0</v>
+        <v>2414</v>
       </c>
       <c r="AT3" t="n">
-        <v>5052.0</v>
+        <v>5052</v>
       </c>
       <c r="AU3" t="n">
-        <v>22690.0</v>
+        <v>22690</v>
       </c>
       <c r="AV3" t="n">
-        <v>5259.0</v>
+        <v>5259</v>
       </c>
       <c r="AW3" t="n">
-        <v>25316.0</v>
+        <v>25316</v>
       </c>
       <c r="AX3" t="n">
-        <v>5693.0</v>
+        <v>5693</v>
       </c>
       <c r="AY3" t="n">
-        <v>6812.0</v>
+        <v>6812</v>
       </c>
       <c r="AZ3" t="n">
-        <v>11169.0</v>
+        <v>11169</v>
       </c>
       <c r="BA3" t="n">
-        <v>24954.0</v>
+        <v>24954</v>
       </c>
       <c r="BB3" t="n">
-        <v>90290.0</v>
+        <v>90290</v>
       </c>
       <c r="BC3" t="n">
-        <v>3898.0</v>
+        <v>3898</v>
       </c>
       <c r="BD3" t="n">
-        <v>30867.0</v>
+        <v>30867</v>
       </c>
       <c r="BE3" t="n">
-        <v>13928.0</v>
+        <v>13928</v>
       </c>
       <c r="BF3" t="n">
-        <v>6735.0</v>
+        <v>6735</v>
       </c>
       <c r="BG3" t="n">
-        <v>5787.0</v>
+        <v>5787</v>
       </c>
       <c r="BH3" t="n">
-        <v>54570.0</v>
+        <v>54570</v>
       </c>
       <c r="BI3" t="n">
-        <v>14576.0</v>
+        <v>14576</v>
       </c>
       <c r="BJ3" t="n">
-        <v>302164.0</v>
+        <v>302164</v>
       </c>
       <c r="BK3" t="n">
-        <v>120980.0</v>
+        <v>120980</v>
       </c>
       <c r="BL3" t="n">
-        <v>32515.0</v>
+        <v>32515</v>
       </c>
       <c r="BM3" t="n">
-        <v>64022.0</v>
+        <v>64022</v>
       </c>
       <c r="BN3" t="n">
-        <v>36420.0</v>
+        <v>36420</v>
       </c>
       <c r="BO3" t="n">
-        <v>6990.0</v>
+        <v>6990</v>
       </c>
       <c r="BP3" t="n">
-        <v>28122.0</v>
+        <v>28122</v>
       </c>
       <c r="BQ3" t="n">
-        <v>40334.0</v>
+        <v>40334</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B4" t="n">
-        <v>18381.0</v>
+        <v>18381</v>
       </c>
       <c r="C4" t="n">
-        <v>12193.0</v>
+        <v>12193</v>
       </c>
       <c r="D4" t="n">
-        <v>1647.0</v>
+        <v>1647</v>
       </c>
       <c r="E4" t="n">
-        <v>2162.0</v>
+        <v>2162</v>
       </c>
       <c r="F4" t="n">
-        <v>8706.0</v>
+        <v>8706</v>
       </c>
       <c r="G4" t="n">
-        <v>2692.0</v>
+        <v>2692</v>
       </c>
       <c r="H4" t="n">
-        <v>1191.0</v>
+        <v>1191</v>
       </c>
       <c r="I4" t="n">
-        <v>10034.0</v>
+        <v>10034</v>
       </c>
       <c r="J4" t="n">
-        <v>4792.0</v>
+        <v>4792</v>
       </c>
       <c r="K4" t="n">
-        <v>12633.0</v>
+        <v>12633</v>
       </c>
       <c r="L4" t="n">
-        <v>3995.0</v>
+        <v>3995</v>
       </c>
       <c r="M4" t="n">
-        <v>867.0</v>
+        <v>867</v>
       </c>
       <c r="N4" t="n">
-        <v>6415.0</v>
+        <v>6415</v>
       </c>
       <c r="O4" t="n">
-        <v>9801.0</v>
+        <v>9801</v>
       </c>
       <c r="P4" t="n">
-        <v>6240.0</v>
+        <v>6240</v>
       </c>
       <c r="Q4" t="n">
-        <v>3781.0</v>
+        <v>3781</v>
       </c>
       <c r="R4" t="n">
-        <v>6051.0</v>
+        <v>6051</v>
       </c>
       <c r="S4" t="n">
-        <v>3339.0</v>
+        <v>3339</v>
       </c>
       <c r="T4" t="n">
-        <v>2903.0</v>
+        <v>2903</v>
       </c>
       <c r="U4" t="n">
-        <v>2040.0</v>
+        <v>2040</v>
       </c>
       <c r="V4" t="n">
-        <v>5042.0</v>
+        <v>5042</v>
       </c>
       <c r="W4" t="n">
-        <v>4355.0</v>
+        <v>4355</v>
       </c>
       <c r="X4" t="n">
-        <v>2810.0</v>
+        <v>2810</v>
       </c>
       <c r="Y4" t="n">
-        <v>4835.0</v>
+        <v>4835</v>
       </c>
       <c r="Z4" t="n">
-        <v>10232.0</v>
+        <v>10232</v>
       </c>
       <c r="AA4" t="n">
-        <v>9445.0</v>
+        <v>9445</v>
       </c>
       <c r="AB4" t="n">
-        <v>6674.0</v>
+        <v>6674</v>
       </c>
       <c r="AC4" t="n">
-        <v>3511.0</v>
+        <v>3511</v>
       </c>
       <c r="AD4" t="n">
-        <v>13239.0</v>
+        <v>13239</v>
       </c>
       <c r="AE4" t="n">
-        <v>6302.0</v>
+        <v>6302</v>
       </c>
       <c r="AF4" t="n">
-        <v>8046.0</v>
+        <v>8046</v>
       </c>
       <c r="AG4" t="n">
-        <v>14403.0</v>
+        <v>14403</v>
       </c>
       <c r="AH4" t="n">
-        <v>11392.0</v>
+        <v>11392</v>
       </c>
       <c r="AI4" t="n">
-        <v>11936.0</v>
+        <v>11936</v>
       </c>
       <c r="AJ4" t="n">
-        <v>4679.0</v>
+        <v>4679</v>
       </c>
       <c r="AK4" t="n">
-        <v>7618.0</v>
+        <v>7618</v>
       </c>
       <c r="AL4" t="n">
-        <v>6060.0</v>
+        <v>6060</v>
       </c>
       <c r="AM4" t="n">
-        <v>9111.0</v>
+        <v>9111</v>
       </c>
       <c r="AN4" t="n">
-        <v>6291.0</v>
+        <v>6291</v>
       </c>
       <c r="AO4" t="n">
-        <v>66155.0</v>
+        <v>66155</v>
       </c>
       <c r="AP4" t="n">
-        <v>22897.0</v>
+        <v>22897</v>
       </c>
       <c r="AQ4" t="n">
-        <v>128144.0</v>
+        <v>128144</v>
       </c>
       <c r="AR4" t="n">
-        <v>35170.0</v>
+        <v>35170</v>
       </c>
       <c r="AS4" t="n">
-        <v>1877.0</v>
+        <v>1877</v>
       </c>
       <c r="AT4" t="n">
-        <v>3843.0</v>
+        <v>3843</v>
       </c>
       <c r="AU4" t="n">
-        <v>17313.0</v>
+        <v>17313</v>
       </c>
       <c r="AV4" t="n">
-        <v>4267.0</v>
+        <v>4267</v>
       </c>
       <c r="AW4" t="n">
-        <v>21550.0</v>
+        <v>21550</v>
       </c>
       <c r="AX4" t="n">
-        <v>4435.0</v>
+        <v>4435</v>
       </c>
       <c r="AY4" t="n">
-        <v>5275.0</v>
+        <v>5275</v>
       </c>
       <c r="AZ4" t="n">
-        <v>8537.0</v>
+        <v>8537</v>
       </c>
       <c r="BA4" t="n">
-        <v>19440.0</v>
+        <v>19440</v>
       </c>
       <c r="BB4" t="n">
-        <v>70303.0</v>
+        <v>70303</v>
       </c>
       <c r="BC4" t="n">
-        <v>3027.0</v>
+        <v>3027</v>
       </c>
       <c r="BD4" t="n">
-        <v>24734.0</v>
+        <v>24734</v>
       </c>
       <c r="BE4" t="n">
-        <v>11142.0</v>
+        <v>11142</v>
       </c>
       <c r="BF4" t="n">
-        <v>5444.0</v>
+        <v>5444</v>
       </c>
       <c r="BG4" t="n">
-        <v>4695.0</v>
+        <v>4695</v>
       </c>
       <c r="BH4" t="n">
-        <v>42523.0</v>
+        <v>42523</v>
       </c>
       <c r="BI4" t="n">
-        <v>11294.0</v>
+        <v>11294</v>
       </c>
       <c r="BJ4" t="n">
-        <v>216062.0</v>
+        <v>216062</v>
       </c>
       <c r="BK4" t="n">
-        <v>104220.0</v>
+        <v>104220</v>
       </c>
       <c r="BL4" t="n">
-        <v>27269.0</v>
+        <v>27269</v>
       </c>
       <c r="BM4" t="n">
-        <v>52938.0</v>
+        <v>52938</v>
       </c>
       <c r="BN4" t="n">
-        <v>29977.0</v>
+        <v>29977</v>
       </c>
       <c r="BO4" t="n">
-        <v>6212.0</v>
+        <v>6212</v>
       </c>
       <c r="BP4" t="n">
-        <v>24311.0</v>
+        <v>24311</v>
       </c>
       <c r="BQ4" t="n">
-        <v>38387.0</v>
+        <v>38387</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" t="n">
-        <v>3206.0</v>
+        <v>3206</v>
       </c>
       <c r="C5" t="n">
-        <v>1869.0</v>
+        <v>1869</v>
       </c>
       <c r="D5" t="n">
-        <v>336.0</v>
+        <v>336</v>
       </c>
       <c r="E5" t="n">
-        <v>610.0</v>
+        <v>610</v>
       </c>
       <c r="F5" t="n">
-        <v>3495.0</v>
+        <v>3495</v>
       </c>
       <c r="G5" t="n">
-        <v>995.0</v>
+        <v>995</v>
       </c>
       <c r="H5" t="n">
-        <v>316.0</v>
+        <v>316</v>
       </c>
       <c r="I5" t="n">
-        <v>3077.0</v>
+        <v>3077</v>
       </c>
       <c r="J5" t="n">
-        <v>1383.0</v>
+        <v>1383</v>
       </c>
       <c r="K5" t="n">
-        <v>3462.0</v>
+        <v>3462</v>
       </c>
       <c r="L5" t="n">
-        <v>1272.0</v>
+        <v>1272</v>
       </c>
       <c r="M5" t="n">
-        <v>281.0</v>
+        <v>281</v>
       </c>
       <c r="N5" t="n">
-        <v>1643.0</v>
+        <v>1643</v>
       </c>
       <c r="O5" t="n">
-        <v>2398.0</v>
+        <v>2398</v>
       </c>
       <c r="P5" t="n">
-        <v>1607.0</v>
+        <v>1607</v>
       </c>
       <c r="Q5" t="n">
-        <v>877.0</v>
+        <v>877</v>
       </c>
       <c r="R5" t="n">
-        <v>1914.0</v>
+        <v>1914</v>
       </c>
       <c r="S5" t="n">
-        <v>878.0</v>
+        <v>878</v>
       </c>
       <c r="T5" t="n">
-        <v>1172.0</v>
+        <v>1172</v>
       </c>
       <c r="U5" t="n">
-        <v>569.0</v>
+        <v>569</v>
       </c>
       <c r="V5" t="n">
-        <v>1696.0</v>
+        <v>1696</v>
       </c>
       <c r="W5" t="n">
-        <v>1487.0</v>
+        <v>1487</v>
       </c>
       <c r="X5" t="n">
-        <v>758.0</v>
+        <v>758</v>
       </c>
       <c r="Y5" t="n">
-        <v>1485.0</v>
+        <v>1485</v>
       </c>
       <c r="Z5" t="n">
-        <v>3080.0</v>
+        <v>3080</v>
       </c>
       <c r="AA5" t="n">
-        <v>2509.0</v>
+        <v>2509</v>
       </c>
       <c r="AB5" t="n">
-        <v>2143.0</v>
+        <v>2143</v>
       </c>
       <c r="AC5" t="n">
-        <v>1068.0</v>
+        <v>1068</v>
       </c>
       <c r="AD5" t="n">
-        <v>3699.0</v>
+        <v>3699</v>
       </c>
       <c r="AE5" t="n">
-        <v>1930.0</v>
+        <v>1930</v>
       </c>
       <c r="AF5" t="n">
-        <v>2411.0</v>
+        <v>2411</v>
       </c>
       <c r="AG5" t="n">
-        <v>4494.0</v>
+        <v>4494</v>
       </c>
       <c r="AH5" t="n">
-        <v>3595.0</v>
+        <v>3595</v>
       </c>
       <c r="AI5" t="n">
-        <v>3573.0</v>
+        <v>3573</v>
       </c>
       <c r="AJ5" t="n">
-        <v>1442.0</v>
+        <v>1442</v>
       </c>
       <c r="AK5" t="n">
-        <v>2034.0</v>
+        <v>2034</v>
       </c>
       <c r="AL5" t="n">
-        <v>1431.0</v>
+        <v>1431</v>
       </c>
       <c r="AM5" t="n">
-        <v>3020.0</v>
+        <v>3020</v>
       </c>
       <c r="AN5" t="n">
-        <v>1815.0</v>
+        <v>1815</v>
       </c>
       <c r="AO5" t="n">
-        <v>15558.0</v>
+        <v>15558</v>
       </c>
       <c r="AP5" t="n">
-        <v>5197.0</v>
+        <v>5197</v>
       </c>
       <c r="AQ5" t="n">
-        <v>33962.0</v>
+        <v>33962</v>
       </c>
       <c r="AR5" t="n">
-        <v>8676.0</v>
+        <v>8676</v>
       </c>
       <c r="AS5" t="n">
-        <v>537.0</v>
+        <v>537</v>
       </c>
       <c r="AT5" t="n">
-        <v>1209.0</v>
+        <v>1209</v>
       </c>
       <c r="AU5" t="n">
-        <v>5377.0</v>
+        <v>5377</v>
       </c>
       <c r="AV5" t="n">
-        <v>992.0</v>
+        <v>992</v>
       </c>
       <c r="AW5" t="n">
-        <v>3766.0</v>
+        <v>3766</v>
       </c>
       <c r="AX5" t="n">
-        <v>1258.0</v>
+        <v>1258</v>
       </c>
       <c r="AY5" t="n">
-        <v>1537.0</v>
+        <v>1537</v>
       </c>
       <c r="AZ5" t="n">
-        <v>2632.0</v>
+        <v>2632</v>
       </c>
       <c r="BA5" t="n">
-        <v>5514.0</v>
+        <v>5514</v>
       </c>
       <c r="BB5" t="n">
-        <v>19987.0</v>
+        <v>19987</v>
       </c>
       <c r="BC5" t="n">
-        <v>871.0</v>
+        <v>871</v>
       </c>
       <c r="BD5" t="n">
-        <v>6133.0</v>
+        <v>6133</v>
       </c>
       <c r="BE5" t="n">
-        <v>2786.0</v>
+        <v>2786</v>
       </c>
       <c r="BF5" t="n">
-        <v>1291.0</v>
+        <v>1291</v>
       </c>
       <c r="BG5" t="n">
-        <v>1092.0</v>
+        <v>1092</v>
       </c>
       <c r="BH5" t="n">
-        <v>12047.0</v>
+        <v>12047</v>
       </c>
       <c r="BI5" t="n">
-        <v>3282.0</v>
+        <v>3282</v>
       </c>
       <c r="BJ5" t="n">
-        <v>41470.0</v>
+        <v>41470</v>
       </c>
       <c r="BK5" t="n">
-        <v>14100.0</v>
+        <v>14100</v>
       </c>
       <c r="BL5" t="n">
-        <v>5246.0</v>
+        <v>5246</v>
       </c>
       <c r="BM5" t="n">
-        <v>7664.0</v>
+        <v>7664</v>
       </c>
       <c r="BN5" t="n">
-        <v>6443.0</v>
+        <v>6443</v>
       </c>
       <c r="BO5" t="n">
-        <v>778.0</v>
+        <v>778</v>
       </c>
       <c r="BP5" t="n">
-        <v>3811.0</v>
+        <v>3811</v>
       </c>
       <c r="BQ5" t="n">
-        <v>1947.0</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B6" t="n">
-        <v>3203.0</v>
+        <v>3203</v>
       </c>
       <c r="C6" t="n">
-        <v>1869.0</v>
+        <v>1869</v>
       </c>
       <c r="D6" t="n">
-        <v>334.0</v>
+        <v>334</v>
       </c>
       <c r="E6" t="n">
-        <v>584.0</v>
+        <v>584</v>
       </c>
       <c r="F6" t="n">
-        <v>2724.0</v>
+        <v>2724</v>
       </c>
       <c r="G6" t="n">
-        <v>861.0</v>
+        <v>861</v>
       </c>
       <c r="H6" t="n">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="I6" t="n">
-        <v>3007.0</v>
+        <v>3007</v>
       </c>
       <c r="J6" t="n">
-        <v>1359.0</v>
+        <v>1359</v>
       </c>
       <c r="K6" t="n">
-        <v>3351.0</v>
+        <v>3351</v>
       </c>
       <c r="L6" t="n">
-        <v>1193.0</v>
+        <v>1193</v>
       </c>
       <c r="M6" t="n">
-        <v>269.0</v>
+        <v>269</v>
       </c>
       <c r="N6" t="n">
-        <v>1631.0</v>
+        <v>1631</v>
       </c>
       <c r="O6" t="n">
-        <v>2388.0</v>
+        <v>2388</v>
       </c>
       <c r="P6" t="n">
-        <v>1595.0</v>
+        <v>1595</v>
       </c>
       <c r="Q6" t="n">
-        <v>868.0</v>
+        <v>868</v>
       </c>
       <c r="R6" t="n">
-        <v>1831.0</v>
+        <v>1831</v>
       </c>
       <c r="S6" t="n">
-        <v>863.0</v>
+        <v>863</v>
       </c>
       <c r="T6" t="n">
-        <v>842.0</v>
+        <v>842</v>
       </c>
       <c r="U6" t="n">
-        <v>549.0</v>
+        <v>549</v>
       </c>
       <c r="V6" t="n">
-        <v>1516.0</v>
+        <v>1516</v>
       </c>
       <c r="W6" t="n">
-        <v>1348.0</v>
+        <v>1348</v>
       </c>
       <c r="X6" t="n">
-        <v>723.0</v>
+        <v>723</v>
       </c>
       <c r="Y6" t="n">
-        <v>1435.0</v>
+        <v>1435</v>
       </c>
       <c r="Z6" t="n">
-        <v>3024.0</v>
+        <v>3024</v>
       </c>
       <c r="AA6" t="n">
-        <v>2452.0</v>
+        <v>2452</v>
       </c>
       <c r="AB6" t="n">
-        <v>2064.0</v>
+        <v>2064</v>
       </c>
       <c r="AC6" t="n">
-        <v>1032.0</v>
+        <v>1032</v>
       </c>
       <c r="AD6" t="n">
-        <v>3629.0</v>
+        <v>3629</v>
       </c>
       <c r="AE6" t="n">
-        <v>1856.0</v>
+        <v>1856</v>
       </c>
       <c r="AF6" t="n">
-        <v>2309.0</v>
+        <v>2309</v>
       </c>
       <c r="AG6" t="n">
-        <v>4346.0</v>
+        <v>4346</v>
       </c>
       <c r="AH6" t="n">
-        <v>3378.0</v>
+        <v>3378</v>
       </c>
       <c r="AI6" t="n">
-        <v>3481.0</v>
+        <v>3481</v>
       </c>
       <c r="AJ6" t="n">
-        <v>1378.0</v>
+        <v>1378</v>
       </c>
       <c r="AK6" t="n">
-        <v>1991.0</v>
+        <v>1991</v>
       </c>
       <c r="AL6" t="n">
-        <v>1386.0</v>
+        <v>1386</v>
       </c>
       <c r="AM6" t="n">
-        <v>2547.0</v>
+        <v>2547</v>
       </c>
       <c r="AN6" t="n">
-        <v>1762.0</v>
+        <v>1762</v>
       </c>
       <c r="AO6" t="n">
-        <v>15085.0</v>
+        <v>15085</v>
       </c>
       <c r="AP6" t="n">
-        <v>5154.0</v>
+        <v>5154</v>
       </c>
       <c r="AQ6" t="n">
-        <v>33445.0</v>
+        <v>33445</v>
       </c>
       <c r="AR6" t="n">
-        <v>8490.0</v>
+        <v>8490</v>
       </c>
       <c r="AS6" t="n">
-        <v>526.0</v>
+        <v>526</v>
       </c>
       <c r="AT6" t="n">
-        <v>1153.0</v>
+        <v>1153</v>
       </c>
       <c r="AU6" t="n">
-        <v>5012.0</v>
+        <v>5012</v>
       </c>
       <c r="AV6" t="n">
-        <v>973.0</v>
+        <v>973</v>
       </c>
       <c r="AW6" t="n">
-        <v>3733.0</v>
+        <v>3733</v>
       </c>
       <c r="AX6" t="n">
-        <v>1189.0</v>
+        <v>1189</v>
       </c>
       <c r="AY6" t="n">
-        <v>1433.0</v>
+        <v>1433</v>
       </c>
       <c r="AZ6" t="n">
-        <v>2409.0</v>
+        <v>2409</v>
       </c>
       <c r="BA6" t="n">
-        <v>5313.0</v>
+        <v>5313</v>
       </c>
       <c r="BB6" t="n">
-        <v>15074.0</v>
+        <v>15074</v>
       </c>
       <c r="BC6" t="n">
-        <v>839.0</v>
+        <v>839</v>
       </c>
       <c r="BD6" t="n">
-        <v>5814.0</v>
+        <v>5814</v>
       </c>
       <c r="BE6" t="n">
-        <v>2740.0</v>
+        <v>2740</v>
       </c>
       <c r="BF6" t="n">
-        <v>1277.0</v>
+        <v>1277</v>
       </c>
       <c r="BG6" t="n">
-        <v>1074.0</v>
+        <v>1074</v>
       </c>
       <c r="BH6" t="n">
-        <v>11878.0</v>
+        <v>11878</v>
       </c>
       <c r="BI6" t="n">
-        <v>3241.0</v>
+        <v>3241</v>
       </c>
       <c r="BJ6" t="n">
-        <v>41242.0</v>
+        <v>41242</v>
       </c>
       <c r="BK6" t="n">
-        <v>14082.0</v>
+        <v>14082</v>
       </c>
       <c r="BL6" t="n">
-        <v>5044.0</v>
+        <v>5044</v>
       </c>
       <c r="BM6" t="n">
-        <v>7663.0</v>
+        <v>7663</v>
       </c>
       <c r="BN6" t="n">
-        <v>6260.0</v>
+        <v>6260</v>
       </c>
       <c r="BO6" t="n">
-        <v>766.0</v>
+        <v>766</v>
       </c>
       <c r="BP6" t="n">
-        <v>3726.0</v>
+        <v>3726</v>
       </c>
       <c r="BQ6" t="n">
-        <v>1947.0</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B7" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="F7" t="n">
-        <v>771.0</v>
+        <v>771</v>
       </c>
       <c r="G7" t="n">
-        <v>134.0</v>
+        <v>134</v>
       </c>
       <c r="H7" t="n">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="I7" t="n">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="J7" t="n">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="K7" t="n">
-        <v>111.0</v>
+        <v>111</v>
       </c>
       <c r="L7" t="n">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="M7" t="n">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="N7" t="n">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="O7" t="n">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="P7" t="n">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q7" t="n">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="R7" t="n">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="S7" t="n">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T7" t="n">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="U7" t="n">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="V7" t="n">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="W7" t="n">
-        <v>139.0</v>
+        <v>139</v>
       </c>
       <c r="X7" t="n">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="Y7" t="n">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="Z7" t="n">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="AA7" t="n">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="AB7" t="n">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="AC7" t="n">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="AD7" t="n">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="AE7" t="n">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="AF7" t="n">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="AG7" t="n">
-        <v>148.0</v>
+        <v>148</v>
       </c>
       <c r="AH7" t="n">
-        <v>217.0</v>
+        <v>217</v>
       </c>
       <c r="AI7" t="n">
-        <v>92.0</v>
+        <v>92</v>
       </c>
       <c r="AJ7" t="n">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="AK7" t="n">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="AL7" t="n">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="AM7" t="n">
-        <v>473.0</v>
+        <v>473</v>
       </c>
       <c r="AN7" t="n">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="AO7" t="n">
-        <v>473.0</v>
+        <v>473</v>
       </c>
       <c r="AP7" t="n">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="AQ7" t="n">
-        <v>517.0</v>
+        <v>517</v>
       </c>
       <c r="AR7" t="n">
-        <v>186.0</v>
+        <v>186</v>
       </c>
       <c r="AS7" t="n">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AT7" t="n">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="AU7" t="n">
-        <v>365.0</v>
+        <v>365</v>
       </c>
       <c r="AV7" t="n">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="AW7" t="n">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="AX7" t="n">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="AY7" t="n">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="AZ7" t="n">
-        <v>223.0</v>
+        <v>223</v>
       </c>
       <c r="BA7" t="n">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="BB7" t="n">
-        <v>4913.0</v>
+        <v>4913</v>
       </c>
       <c r="BC7" t="n">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="BD7" t="n">
-        <v>319.0</v>
+        <v>319</v>
       </c>
       <c r="BE7" t="n">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="BF7" t="n">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="BG7" t="n">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="BH7" t="n">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="BI7" t="n">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="BJ7" t="n">
-        <v>228.0</v>
+        <v>228</v>
       </c>
       <c r="BK7" t="n">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="BL7" t="n">
-        <v>202.0</v>
+        <v>202</v>
       </c>
       <c r="BM7" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="BN7" t="n">
-        <v>183.0</v>
+        <v>183</v>
       </c>
       <c r="BO7" t="n">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="BP7" t="n">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="BQ7" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AQ8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AR8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AS8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AW8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AX8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AY8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AZ8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BA8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BB8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BC8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BD8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BE8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BF8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BH8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BJ8" t="n">
-        <v>44632.0</v>
+        <v>44632</v>
       </c>
       <c r="BK8" t="n">
-        <v>2660.0</v>
+        <v>2660</v>
       </c>
       <c r="BL8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BM8" t="n">
-        <v>3420.0</v>
+        <v>3420</v>
       </c>
       <c r="BN8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BP8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BQ8" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
-        <v>79479.0</v>
+        <v>79479</v>
       </c>
       <c r="C9" t="n">
-        <v>30528.0</v>
+        <v>30528</v>
       </c>
       <c r="D9" t="n">
-        <v>12899.0</v>
+        <v>12899</v>
       </c>
       <c r="E9" t="n">
-        <v>3710.0</v>
+        <v>3710</v>
       </c>
       <c r="F9" t="n">
-        <v>50581.0</v>
+        <v>50581</v>
       </c>
       <c r="G9" t="n">
-        <v>32474.0</v>
+        <v>32474</v>
       </c>
       <c r="H9" t="n">
-        <v>1827.0</v>
+        <v>1827</v>
       </c>
       <c r="I9" t="n">
-        <v>6779.0</v>
+        <v>6779</v>
       </c>
       <c r="J9" t="n">
-        <v>2911.0</v>
+        <v>2911</v>
       </c>
       <c r="K9" t="n">
-        <v>10226.0</v>
+        <v>10226</v>
       </c>
       <c r="L9" t="n">
-        <v>11443.0</v>
+        <v>11443</v>
       </c>
       <c r="M9" t="n">
-        <v>2366.0</v>
+        <v>2366</v>
       </c>
       <c r="N9" t="n">
-        <v>2574.0</v>
+        <v>2574</v>
       </c>
       <c r="O9" t="n">
-        <v>9449.0</v>
+        <v>9449</v>
       </c>
       <c r="P9" t="n">
-        <v>2433.0</v>
+        <v>2433</v>
       </c>
       <c r="Q9" t="n">
-        <v>3662.0</v>
+        <v>3662</v>
       </c>
       <c r="R9" t="n">
-        <v>6959.0</v>
+        <v>6959</v>
       </c>
       <c r="S9" t="n">
-        <v>3102.0</v>
+        <v>3102</v>
       </c>
       <c r="T9" t="n">
-        <v>11680.0</v>
+        <v>11680</v>
       </c>
       <c r="U9" t="n">
-        <v>2581.0</v>
+        <v>2581</v>
       </c>
       <c r="V9" t="n">
-        <v>7163.0</v>
+        <v>7163</v>
       </c>
       <c r="W9" t="n">
-        <v>2884.0</v>
+        <v>2884</v>
       </c>
       <c r="X9" t="n">
-        <v>3378.0</v>
+        <v>3378</v>
       </c>
       <c r="Y9" t="n">
-        <v>12905.0</v>
+        <v>12905</v>
       </c>
       <c r="Z9" t="n">
-        <v>7412.0</v>
+        <v>7412</v>
       </c>
       <c r="AA9" t="n">
-        <v>9890.0</v>
+        <v>9890</v>
       </c>
       <c r="AB9" t="n">
-        <v>7531.0</v>
+        <v>7531</v>
       </c>
       <c r="AC9" t="n">
-        <v>2431.0</v>
+        <v>2431</v>
       </c>
       <c r="AD9" t="n">
-        <v>11795.0</v>
+        <v>11795</v>
       </c>
       <c r="AE9" t="n">
-        <v>5134.0</v>
+        <v>5134</v>
       </c>
       <c r="AF9" t="n">
-        <v>3713.0</v>
+        <v>3713</v>
       </c>
       <c r="AG9" t="n">
-        <v>11192.0</v>
+        <v>11192</v>
       </c>
       <c r="AH9" t="n">
-        <v>22229.0</v>
+        <v>22229</v>
       </c>
       <c r="AI9" t="n">
-        <v>7692.0</v>
+        <v>7692</v>
       </c>
       <c r="AJ9" t="n">
-        <v>3306.0</v>
+        <v>3306</v>
       </c>
       <c r="AK9" t="n">
-        <v>13484.0</v>
+        <v>13484</v>
       </c>
       <c r="AL9" t="n">
-        <v>9423.0</v>
+        <v>9423</v>
       </c>
       <c r="AM9" t="n">
-        <v>55638.0</v>
+        <v>55638</v>
       </c>
       <c r="AN9" t="n">
-        <v>15591.0</v>
+        <v>15591</v>
       </c>
       <c r="AO9" t="n">
-        <v>122636.0</v>
+        <v>122636</v>
       </c>
       <c r="AP9" t="n">
-        <v>36887.0</v>
+        <v>36887</v>
       </c>
       <c r="AQ9" t="n">
-        <v>183234.0</v>
+        <v>183234</v>
       </c>
       <c r="AR9" t="n">
-        <v>47765.0</v>
+        <v>47765</v>
       </c>
       <c r="AS9" t="n">
-        <v>912.0</v>
+        <v>912</v>
       </c>
       <c r="AT9" t="n">
-        <v>882.0</v>
+        <v>882</v>
       </c>
       <c r="AU9" t="n">
-        <v>15115.0</v>
+        <v>15115</v>
       </c>
       <c r="AV9" t="n">
-        <v>3089.0</v>
+        <v>3089</v>
       </c>
       <c r="AW9" t="n">
-        <v>35720.0</v>
+        <v>35720</v>
       </c>
       <c r="AX9" t="n">
-        <v>4649.0</v>
+        <v>4649</v>
       </c>
       <c r="AY9" t="n">
-        <v>4763.0</v>
+        <v>4763</v>
       </c>
       <c r="AZ9" t="n">
-        <v>44052.0</v>
+        <v>44052</v>
       </c>
       <c r="BA9" t="n">
-        <v>19821.0</v>
+        <v>19821</v>
       </c>
       <c r="BB9" t="n">
-        <v>130442.0</v>
+        <v>130442</v>
       </c>
       <c r="BC9" t="n">
-        <v>270357.0</v>
+        <v>270357</v>
       </c>
       <c r="BD9" t="n">
-        <v>45960.0</v>
+        <v>45960</v>
       </c>
       <c r="BE9" t="n">
-        <v>16322.0</v>
+        <v>16322</v>
       </c>
       <c r="BF9" t="n">
-        <v>12337.0</v>
+        <v>12337</v>
       </c>
       <c r="BG9" t="n">
-        <v>10088.0</v>
+        <v>10088</v>
       </c>
       <c r="BH9" t="n">
-        <v>29379.0</v>
+        <v>29379</v>
       </c>
       <c r="BI9" t="n">
-        <v>1977.0</v>
+        <v>1977</v>
       </c>
       <c r="BJ9" t="n">
-        <v>41139.0</v>
+        <v>41139</v>
       </c>
       <c r="BK9" t="n">
-        <v>6173.0</v>
+        <v>6173</v>
       </c>
       <c r="BL9" t="n">
-        <v>3370.0</v>
+        <v>3370</v>
       </c>
       <c r="BM9" t="n">
-        <v>3347.0</v>
+        <v>3347</v>
       </c>
       <c r="BN9" t="n">
-        <v>24646.0</v>
+        <v>24646</v>
       </c>
       <c r="BO9" t="n">
-        <v>7186.0</v>
+        <v>7186</v>
       </c>
       <c r="BP9" t="n">
-        <v>19060.0</v>
+        <v>19060</v>
       </c>
       <c r="BQ9" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B10" t="n">
-        <v>45811.0</v>
+        <v>45811</v>
       </c>
       <c r="C10" t="n">
-        <v>21852.0</v>
+        <v>21852</v>
       </c>
       <c r="D10" t="n">
-        <v>5657.0</v>
+        <v>5657</v>
       </c>
       <c r="E10" t="n">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>244.0</v>
+        <v>244</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2527.0</v>
+        <v>2527</v>
       </c>
       <c r="L10" t="n">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>734.0</v>
+        <v>734</v>
       </c>
       <c r="O10" t="n">
-        <v>6034.0</v>
+        <v>6034</v>
       </c>
       <c r="P10" t="n">
-        <v>581.0</v>
+        <v>581</v>
       </c>
       <c r="Q10" t="n">
-        <v>1358.0</v>
+        <v>1358</v>
       </c>
       <c r="R10" t="n">
-        <v>206.0</v>
+        <v>206</v>
       </c>
       <c r="S10" t="n">
-        <v>491.0</v>
+        <v>491</v>
       </c>
       <c r="T10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>153.0</v>
+        <v>153</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>218.0</v>
+        <v>218</v>
       </c>
       <c r="AA10" t="n">
-        <v>682.0</v>
+        <v>682</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>1744.0</v>
+        <v>1744</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AI10" t="n">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="AJ10" t="n">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="AK10" t="n">
-        <v>1515.0</v>
+        <v>1515</v>
       </c>
       <c r="AL10" t="n">
-        <v>4384.0</v>
+        <v>4384</v>
       </c>
       <c r="AM10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AN10" t="n">
-        <v>1323.0</v>
+        <v>1323</v>
       </c>
       <c r="AO10" t="n">
-        <v>44580.0</v>
+        <v>44580</v>
       </c>
       <c r="AP10" t="n">
-        <v>15444.0</v>
+        <v>15444</v>
       </c>
       <c r="AQ10" t="n">
-        <v>44392.0</v>
+        <v>44392</v>
       </c>
       <c r="AR10" t="n">
-        <v>18905.0</v>
+        <v>18905</v>
       </c>
       <c r="AS10" t="n">
-        <v>121.0</v>
+        <v>121</v>
       </c>
       <c r="AT10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AU10" t="n">
-        <v>911.0</v>
+        <v>911</v>
       </c>
       <c r="AV10" t="n">
-        <v>804.0</v>
+        <v>804</v>
       </c>
       <c r="AW10" t="n">
-        <v>20501.0</v>
+        <v>20501</v>
       </c>
       <c r="AX10" t="n">
-        <v>602.0</v>
+        <v>602</v>
       </c>
       <c r="AY10" t="n">
-        <v>338.0</v>
+        <v>338</v>
       </c>
       <c r="AZ10" t="n">
-        <v>434.0</v>
+        <v>434</v>
       </c>
       <c r="BA10" t="n">
-        <v>4584.0</v>
+        <v>4584</v>
       </c>
       <c r="BB10" t="n">
-        <v>1631.0</v>
+        <v>1631</v>
       </c>
       <c r="BC10" t="n">
-        <v>3973.0</v>
+        <v>3973</v>
       </c>
       <c r="BD10" t="n">
-        <v>22853.0</v>
+        <v>22853</v>
       </c>
       <c r="BE10" t="n">
-        <v>7166.0</v>
+        <v>7166</v>
       </c>
       <c r="BF10" t="n">
-        <v>4668.0</v>
+        <v>4668</v>
       </c>
       <c r="BG10" t="n">
-        <v>709.0</v>
+        <v>709</v>
       </c>
       <c r="BH10" t="n">
-        <v>3333.0</v>
+        <v>3333</v>
       </c>
       <c r="BI10" t="n">
-        <v>680.0</v>
+        <v>680</v>
       </c>
       <c r="BJ10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BK10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BL10" t="n">
-        <v>3124.0</v>
+        <v>3124</v>
       </c>
       <c r="BM10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BN10" t="n">
-        <v>15984.0</v>
+        <v>15984</v>
       </c>
       <c r="BO10" t="n">
-        <v>4542.0</v>
+        <v>4542</v>
       </c>
       <c r="BP10" t="n">
-        <v>14801.0</v>
+        <v>14801</v>
       </c>
       <c r="BQ10" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B11" t="n">
-        <v>33668.0</v>
+        <v>33668</v>
       </c>
       <c r="C11" t="n">
-        <v>8676.0</v>
+        <v>8676</v>
       </c>
       <c r="D11" t="n">
-        <v>7242.0</v>
+        <v>7242</v>
       </c>
       <c r="E11" t="n">
-        <v>3541.0</v>
+        <v>3541</v>
       </c>
       <c r="F11" t="n">
-        <v>50581.0</v>
+        <v>50581</v>
       </c>
       <c r="G11" t="n">
-        <v>32474.0</v>
+        <v>32474</v>
       </c>
       <c r="H11" t="n">
-        <v>1827.0</v>
+        <v>1827</v>
       </c>
       <c r="I11" t="n">
-        <v>6535.0</v>
+        <v>6535</v>
       </c>
       <c r="J11" t="n">
-        <v>2911.0</v>
+        <v>2911</v>
       </c>
       <c r="K11" t="n">
-        <v>7699.0</v>
+        <v>7699</v>
       </c>
       <c r="L11" t="n">
-        <v>11424.0</v>
+        <v>11424</v>
       </c>
       <c r="M11" t="n">
-        <v>2366.0</v>
+        <v>2366</v>
       </c>
       <c r="N11" t="n">
-        <v>1840.0</v>
+        <v>1840</v>
       </c>
       <c r="O11" t="n">
-        <v>3415.0</v>
+        <v>3415</v>
       </c>
       <c r="P11" t="n">
-        <v>1852.0</v>
+        <v>1852</v>
       </c>
       <c r="Q11" t="n">
-        <v>2304.0</v>
+        <v>2304</v>
       </c>
       <c r="R11" t="n">
-        <v>6753.0</v>
+        <v>6753</v>
       </c>
       <c r="S11" t="n">
-        <v>2611.0</v>
+        <v>2611</v>
       </c>
       <c r="T11" t="n">
-        <v>11680.0</v>
+        <v>11680</v>
       </c>
       <c r="U11" t="n">
-        <v>2581.0</v>
+        <v>2581</v>
       </c>
       <c r="V11" t="n">
-        <v>7163.0</v>
+        <v>7163</v>
       </c>
       <c r="W11" t="n">
-        <v>2884.0</v>
+        <v>2884</v>
       </c>
       <c r="X11" t="n">
-        <v>3225.0</v>
+        <v>3225</v>
       </c>
       <c r="Y11" t="n">
-        <v>12905.0</v>
+        <v>12905</v>
       </c>
       <c r="Z11" t="n">
-        <v>7194.0</v>
+        <v>7194</v>
       </c>
       <c r="AA11" t="n">
-        <v>9208.0</v>
+        <v>9208</v>
       </c>
       <c r="AB11" t="n">
-        <v>7531.0</v>
+        <v>7531</v>
       </c>
       <c r="AC11" t="n">
-        <v>2431.0</v>
+        <v>2431</v>
       </c>
       <c r="AD11" t="n">
-        <v>10051.0</v>
+        <v>10051</v>
       </c>
       <c r="AE11" t="n">
-        <v>5134.0</v>
+        <v>5134</v>
       </c>
       <c r="AF11" t="n">
-        <v>3713.0</v>
+        <v>3713</v>
       </c>
       <c r="AG11" t="n">
-        <v>11192.0</v>
+        <v>11192</v>
       </c>
       <c r="AH11" t="n">
-        <v>22229.0</v>
+        <v>22229</v>
       </c>
       <c r="AI11" t="n">
-        <v>7636.0</v>
+        <v>7636</v>
       </c>
       <c r="AJ11" t="n">
-        <v>3272.0</v>
+        <v>3272</v>
       </c>
       <c r="AK11" t="n">
-        <v>11969.0</v>
+        <v>11969</v>
       </c>
       <c r="AL11" t="n">
-        <v>5039.0</v>
+        <v>5039</v>
       </c>
       <c r="AM11" t="n">
-        <v>55638.0</v>
+        <v>55638</v>
       </c>
       <c r="AN11" t="n">
-        <v>14268.0</v>
+        <v>14268</v>
       </c>
       <c r="AO11" t="n">
-        <v>78056.0</v>
+        <v>78056</v>
       </c>
       <c r="AP11" t="n">
-        <v>21443.0</v>
+        <v>21443</v>
       </c>
       <c r="AQ11" t="n">
-        <v>138842.0</v>
+        <v>138842</v>
       </c>
       <c r="AR11" t="n">
-        <v>28860.0</v>
+        <v>28860</v>
       </c>
       <c r="AS11" t="n">
-        <v>791.0</v>
+        <v>791</v>
       </c>
       <c r="AT11" t="n">
-        <v>882.0</v>
+        <v>882</v>
       </c>
       <c r="AU11" t="n">
-        <v>14204.0</v>
+        <v>14204</v>
       </c>
       <c r="AV11" t="n">
-        <v>2285.0</v>
+        <v>2285</v>
       </c>
       <c r="AW11" t="n">
-        <v>15219.0</v>
+        <v>15219</v>
       </c>
       <c r="AX11" t="n">
-        <v>4047.0</v>
+        <v>4047</v>
       </c>
       <c r="AY11" t="n">
-        <v>4425.0</v>
+        <v>4425</v>
       </c>
       <c r="AZ11" t="n">
-        <v>43618.0</v>
+        <v>43618</v>
       </c>
       <c r="BA11" t="n">
-        <v>15237.0</v>
+        <v>15237</v>
       </c>
       <c r="BB11" t="n">
-        <v>128811.0</v>
+        <v>128811</v>
       </c>
       <c r="BC11" t="n">
-        <v>266384.0</v>
+        <v>266384</v>
       </c>
       <c r="BD11" t="n">
-        <v>23107.0</v>
+        <v>23107</v>
       </c>
       <c r="BE11" t="n">
-        <v>9156.0</v>
+        <v>9156</v>
       </c>
       <c r="BF11" t="n">
-        <v>7669.0</v>
+        <v>7669</v>
       </c>
       <c r="BG11" t="n">
-        <v>9379.0</v>
+        <v>9379</v>
       </c>
       <c r="BH11" t="n">
-        <v>26046.0</v>
+        <v>26046</v>
       </c>
       <c r="BI11" t="n">
-        <v>1297.0</v>
+        <v>1297</v>
       </c>
       <c r="BJ11" t="n">
-        <v>41139.0</v>
+        <v>41139</v>
       </c>
       <c r="BK11" t="n">
-        <v>6173.0</v>
+        <v>6173</v>
       </c>
       <c r="BL11" t="n">
-        <v>246.0</v>
+        <v>246</v>
       </c>
       <c r="BM11" t="n">
-        <v>3347.0</v>
+        <v>3347</v>
       </c>
       <c r="BN11" t="n">
-        <v>8662.0</v>
+        <v>8662</v>
       </c>
       <c r="BO11" t="n">
-        <v>2644.0</v>
+        <v>2644</v>
       </c>
       <c r="BP11" t="n">
-        <v>4259.0</v>
+        <v>4259</v>
       </c>
       <c r="BQ11" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B12" t="n">
-        <v>445.0</v>
+        <v>445</v>
       </c>
       <c r="C12" t="n">
-        <v>277.0</v>
+        <v>277</v>
       </c>
       <c r="D12" t="n">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="E12" t="n">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="F12" t="n">
-        <v>692.0</v>
+        <v>692</v>
       </c>
       <c r="G12" t="n">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="H12" t="n">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="I12" t="n">
-        <v>959.0</v>
+        <v>959</v>
       </c>
       <c r="J12" t="n">
-        <v>459.0</v>
+        <v>459</v>
       </c>
       <c r="K12" t="n">
-        <v>1164.0</v>
+        <v>1164</v>
       </c>
       <c r="L12" t="n">
-        <v>514.0</v>
+        <v>514</v>
       </c>
       <c r="M12" t="n">
-        <v>81.0</v>
+        <v>81</v>
       </c>
       <c r="N12" t="n">
-        <v>318.0</v>
+        <v>318</v>
       </c>
       <c r="O12" t="n">
-        <v>379.0</v>
+        <v>379</v>
       </c>
       <c r="P12" t="n">
-        <v>273.0</v>
+        <v>273</v>
       </c>
       <c r="Q12" t="n">
-        <v>216.0</v>
+        <v>216</v>
       </c>
       <c r="R12" t="n">
-        <v>410.0</v>
+        <v>410</v>
       </c>
       <c r="S12" t="n">
-        <v>199.0</v>
+        <v>199</v>
       </c>
       <c r="T12" t="n">
-        <v>574.0</v>
+        <v>574</v>
       </c>
       <c r="U12" t="n">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="V12" t="n">
-        <v>529.0</v>
+        <v>529</v>
       </c>
       <c r="W12" t="n">
-        <v>302.0</v>
+        <v>302</v>
       </c>
       <c r="X12" t="n">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="Y12" t="n">
-        <v>301.0</v>
+        <v>301</v>
       </c>
       <c r="Z12" t="n">
-        <v>598.0</v>
+        <v>598</v>
       </c>
       <c r="AA12" t="n">
-        <v>504.0</v>
+        <v>504</v>
       </c>
       <c r="AB12" t="n">
-        <v>583.0</v>
+        <v>583</v>
       </c>
       <c r="AC12" t="n">
-        <v>259.0</v>
+        <v>259</v>
       </c>
       <c r="AD12" t="n">
-        <v>668.0</v>
+        <v>668</v>
       </c>
       <c r="AE12" t="n">
-        <v>592.0</v>
+        <v>592</v>
       </c>
       <c r="AF12" t="n">
-        <v>471.0</v>
+        <v>471</v>
       </c>
       <c r="AG12" t="n">
-        <v>816.0</v>
+        <v>816</v>
       </c>
       <c r="AH12" t="n">
-        <v>975.0</v>
+        <v>975</v>
       </c>
       <c r="AI12" t="n">
-        <v>674.0</v>
+        <v>674</v>
       </c>
       <c r="AJ12" t="n">
-        <v>257.0</v>
+        <v>257</v>
       </c>
       <c r="AK12" t="n">
-        <v>366.0</v>
+        <v>366</v>
       </c>
       <c r="AL12" t="n">
-        <v>211.0</v>
+        <v>211</v>
       </c>
       <c r="AM12" t="n">
-        <v>1099.0</v>
+        <v>1099</v>
       </c>
       <c r="AN12" t="n">
-        <v>349.0</v>
+        <v>349</v>
       </c>
       <c r="AO12" t="n">
-        <v>2578.0</v>
+        <v>2578</v>
       </c>
       <c r="AP12" t="n">
-        <v>776.0</v>
+        <v>776</v>
       </c>
       <c r="AQ12" t="n">
-        <v>5132.0</v>
+        <v>5132</v>
       </c>
       <c r="AR12" t="n">
-        <v>1539.0</v>
+        <v>1539</v>
       </c>
       <c r="AS12" t="n">
-        <v>179.0</v>
+        <v>179</v>
       </c>
       <c r="AT12" t="n">
-        <v>323.0</v>
+        <v>323</v>
       </c>
       <c r="AU12" t="n">
-        <v>943.0</v>
+        <v>943</v>
       </c>
       <c r="AV12" t="n">
-        <v>171.0</v>
+        <v>171</v>
       </c>
       <c r="AW12" t="n">
-        <v>649.0</v>
+        <v>649</v>
       </c>
       <c r="AX12" t="n">
-        <v>207.0</v>
+        <v>207</v>
       </c>
       <c r="AY12" t="n">
-        <v>727.0</v>
+        <v>727</v>
       </c>
       <c r="AZ12" t="n">
-        <v>2950.0</v>
+        <v>2950</v>
       </c>
       <c r="BA12" t="n">
-        <v>745.0</v>
+        <v>745</v>
       </c>
       <c r="BB12" t="n">
-        <v>3829.0</v>
+        <v>3829</v>
       </c>
       <c r="BC12" t="n">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="BD12" t="n">
-        <v>933.0</v>
+        <v>933</v>
       </c>
       <c r="BE12" t="n">
-        <v>376.0</v>
+        <v>376</v>
       </c>
       <c r="BF12" t="n">
-        <v>213.0</v>
+        <v>213</v>
       </c>
       <c r="BG12" t="n">
-        <v>231.0</v>
+        <v>231</v>
       </c>
       <c r="BH12" t="n">
-        <v>1625.0</v>
+        <v>1625</v>
       </c>
       <c r="BI12" t="n">
-        <v>437.0</v>
+        <v>437</v>
       </c>
       <c r="BJ12" t="n">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="BK12" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="BL12" t="n">
-        <v>945.0</v>
+        <v>945</v>
       </c>
       <c r="BM12" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BN12" t="n">
-        <v>1118.0</v>
+        <v>1118</v>
       </c>
       <c r="BO12" t="n">
-        <v>136.0</v>
+        <v>136</v>
       </c>
       <c r="BP12" t="n">
-        <v>729.0</v>
+        <v>729</v>
       </c>
       <c r="BQ12" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B13" t="n">
-        <v>-1400.0</v>
+        <v>-1400</v>
       </c>
       <c r="C13" t="n">
-        <v>-4.0</v>
+        <v>-4</v>
       </c>
       <c r="D13" t="n">
-        <v>-9.0</v>
+        <v>-9</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AJ13" t="n">
-        <v>-235.0</v>
+        <v>-235</v>
       </c>
       <c r="AK13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AL13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AM13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AN13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AO13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AP13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AQ13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AR13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AS13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AT13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AU13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AV13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AW13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AX13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AY13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AZ13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BA13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BB13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BC13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BD13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BE13" t="n">
-        <v>-623.0</v>
+        <v>-623</v>
       </c>
       <c r="BF13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BG13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BH13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BI13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BJ13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BK13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BL13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BM13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BN13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BO13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BP13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="BQ13" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B14" t="n">
-        <v>168861.0</v>
+        <v>168861</v>
       </c>
       <c r="C14" t="n">
-        <v>83448.0</v>
+        <v>83448</v>
       </c>
       <c r="D14" t="n">
-        <v>20332.0</v>
+        <v>20332</v>
       </c>
       <c r="E14" t="n">
-        <v>14838.0</v>
+        <v>14838</v>
       </c>
       <c r="F14" t="n">
-        <v>117330.0</v>
+        <v>117330</v>
       </c>
       <c r="G14" t="n">
-        <v>56525.0</v>
+        <v>56525</v>
       </c>
       <c r="H14" t="n">
-        <v>9864.0</v>
+        <v>9864</v>
       </c>
       <c r="I14" t="n">
-        <v>137527.0</v>
+        <v>137527</v>
       </c>
       <c r="J14" t="n">
-        <v>44422.0</v>
+        <v>44422</v>
       </c>
       <c r="K14" t="n">
-        <v>153990.0</v>
+        <v>153990</v>
       </c>
       <c r="L14" t="n">
-        <v>53034.0</v>
+        <v>53034</v>
       </c>
       <c r="M14" t="n">
-        <v>13405.0</v>
+        <v>13405</v>
       </c>
       <c r="N14" t="n">
-        <v>40495.0</v>
+        <v>40495</v>
       </c>
       <c r="O14" t="n">
-        <v>48493.0</v>
+        <v>48493</v>
       </c>
       <c r="P14" t="n">
-        <v>29273.0</v>
+        <v>29273</v>
       </c>
       <c r="Q14" t="n">
-        <v>21017.0</v>
+        <v>21017</v>
       </c>
       <c r="R14" t="n">
-        <v>56231.0</v>
+        <v>56231</v>
       </c>
       <c r="S14" t="n">
-        <v>17323.0</v>
+        <v>17323</v>
       </c>
       <c r="T14" t="n">
-        <v>226943.0</v>
+        <v>226943</v>
       </c>
       <c r="U14" t="n">
-        <v>24324.0</v>
+        <v>24324</v>
       </c>
       <c r="V14" t="n">
-        <v>88947.0</v>
+        <v>88947</v>
       </c>
       <c r="W14" t="n">
-        <v>47079.0</v>
+        <v>47079</v>
       </c>
       <c r="X14" t="n">
-        <v>26590.0</v>
+        <v>26590</v>
       </c>
       <c r="Y14" t="n">
-        <v>40773.0</v>
+        <v>40773</v>
       </c>
       <c r="Z14" t="n">
-        <v>72642.0</v>
+        <v>72642</v>
       </c>
       <c r="AA14" t="n">
-        <v>64127.0</v>
+        <v>64127</v>
       </c>
       <c r="AB14" t="n">
-        <v>91530.0</v>
+        <v>91530</v>
       </c>
       <c r="AC14" t="n">
-        <v>37782.0</v>
+        <v>37782</v>
       </c>
       <c r="AD14" t="n">
-        <v>75909.0</v>
+        <v>75909</v>
       </c>
       <c r="AE14" t="n">
-        <v>64420.0</v>
+        <v>64420</v>
       </c>
       <c r="AF14" t="n">
-        <v>58616.0</v>
+        <v>58616</v>
       </c>
       <c r="AG14" t="n">
-        <v>98091.0</v>
+        <v>98091</v>
       </c>
       <c r="AH14" t="n">
-        <v>156859.0</v>
+        <v>156859</v>
       </c>
       <c r="AI14" t="n">
-        <v>80869.0</v>
+        <v>80869</v>
       </c>
       <c r="AJ14" t="n">
-        <v>32916.0</v>
+        <v>32916</v>
       </c>
       <c r="AK14" t="n">
-        <v>50603.0</v>
+        <v>50603</v>
       </c>
       <c r="AL14" t="n">
-        <v>42258.0</v>
+        <v>42258</v>
       </c>
       <c r="AM14" t="n">
-        <v>152676.0</v>
+        <v>152676</v>
       </c>
       <c r="AN14" t="n">
-        <v>43036.0</v>
+        <v>43036</v>
       </c>
       <c r="AO14" t="n">
-        <v>447138.0</v>
+        <v>447138</v>
       </c>
       <c r="AP14" t="n">
-        <v>107309.0</v>
+        <v>107309</v>
       </c>
       <c r="AQ14" t="n">
-        <v>539367.0</v>
+        <v>539367</v>
       </c>
       <c r="AR14" t="n">
-        <v>212091.0</v>
+        <v>212091</v>
       </c>
       <c r="AS14" t="n">
-        <v>10689.0</v>
+        <v>10689</v>
       </c>
       <c r="AT14" t="n">
-        <v>24950.0</v>
+        <v>24950</v>
       </c>
       <c r="AU14" t="n">
-        <v>67559.0</v>
+        <v>67559</v>
       </c>
       <c r="AV14" t="n">
-        <v>15069.0</v>
+        <v>15069</v>
       </c>
       <c r="AW14" t="n">
-        <v>125593.0</v>
+        <v>125593</v>
       </c>
       <c r="AX14" t="n">
-        <v>22843.0</v>
+        <v>22843</v>
       </c>
       <c r="AY14" t="n">
-        <v>28175.0</v>
+        <v>28175</v>
       </c>
       <c r="AZ14" t="n">
-        <v>132637.0</v>
+        <v>132637</v>
       </c>
       <c r="BA14" t="n">
-        <v>67574.0</v>
+        <v>67574</v>
       </c>
       <c r="BB14" t="n">
-        <v>362692.0</v>
+        <v>362692</v>
       </c>
       <c r="BC14" t="n">
-        <v>296205.0</v>
+        <v>296205</v>
       </c>
       <c r="BD14" t="n">
-        <v>114052.0</v>
+        <v>114052</v>
       </c>
       <c r="BE14" t="n">
-        <v>46863.0</v>
+        <v>46863</v>
       </c>
       <c r="BF14" t="n">
-        <v>58081.0</v>
+        <v>58081</v>
       </c>
       <c r="BG14" t="n">
-        <v>25264.0</v>
+        <v>25264</v>
       </c>
       <c r="BH14" t="n">
-        <v>124594.0</v>
+        <v>124594</v>
       </c>
       <c r="BI14" t="n">
-        <v>20741.0</v>
+        <v>20741</v>
       </c>
       <c r="BJ14" t="n">
-        <v>484385.0</v>
+        <v>484385</v>
       </c>
       <c r="BK14" t="n">
-        <v>159171.0</v>
+        <v>159171</v>
       </c>
       <c r="BL14" t="n">
-        <v>57025.0</v>
+        <v>57025</v>
       </c>
       <c r="BM14" t="n">
-        <v>103352.0</v>
+        <v>103352</v>
       </c>
       <c r="BN14" t="n">
-        <v>114420.0</v>
+        <v>114420</v>
       </c>
       <c r="BO14" t="n">
-        <v>23299.0</v>
+        <v>23299</v>
       </c>
       <c r="BP14" t="n">
-        <v>104279.0</v>
+        <v>104279</v>
       </c>
       <c r="BQ14" t="n">
-        <v>40334.0</v>
+        <v>40334</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B15" t="n">
-        <v>6965949.0</v>
+        <v>6965949</v>
       </c>
       <c r="C15" t="n">
-        <v>7473681.0</v>
+        <v>7473681</v>
       </c>
       <c r="D15" t="n">
-        <v>1041304.0</v>
+        <v>1041304</v>
       </c>
       <c r="E15" t="n">
-        <v>138960.0</v>
+        <v>138960</v>
       </c>
       <c r="F15" t="n">
-        <v>60278.0</v>
+        <v>60278</v>
       </c>
       <c r="G15" t="n">
-        <v>35928.0</v>
+        <v>35928</v>
       </c>
       <c r="H15" t="n">
-        <v>31775.0</v>
+        <v>31775</v>
       </c>
       <c r="I15" t="n">
-        <v>638392.0</v>
+        <v>638392</v>
       </c>
       <c r="J15" t="n">
-        <v>228655.0</v>
+        <v>228655</v>
       </c>
       <c r="K15" t="n">
-        <v>1115497.0</v>
+        <v>1115497</v>
       </c>
       <c r="L15" t="n">
-        <v>161508.0</v>
+        <v>161508</v>
       </c>
       <c r="M15" t="n">
-        <v>19343.0</v>
+        <v>19343</v>
       </c>
       <c r="N15" t="n">
-        <v>623594.0</v>
+        <v>623594</v>
       </c>
       <c r="O15" t="n">
-        <v>1748306.0</v>
+        <v>1748306</v>
       </c>
       <c r="P15" t="n">
-        <v>586106.0</v>
+        <v>586106</v>
       </c>
       <c r="Q15" t="n">
-        <v>469599.0</v>
+        <v>469599</v>
       </c>
       <c r="R15" t="n">
-        <v>198663.0</v>
+        <v>198663</v>
       </c>
       <c r="S15" t="n">
-        <v>211376.0</v>
+        <v>211376</v>
       </c>
       <c r="T15" t="n">
-        <v>23984.0</v>
+        <v>23984</v>
       </c>
       <c r="U15" t="n">
-        <v>88492.0</v>
+        <v>88492</v>
       </c>
       <c r="V15" t="n">
-        <v>86072.0</v>
+        <v>86072</v>
       </c>
       <c r="W15" t="n">
-        <v>92165.0</v>
+        <v>92165</v>
       </c>
       <c r="X15" t="n">
-        <v>186165.0</v>
+        <v>186165</v>
       </c>
       <c r="Y15" t="n">
-        <v>98575.0</v>
+        <v>98575</v>
       </c>
       <c r="Z15" t="n">
-        <v>464784.0</v>
+        <v>464784</v>
       </c>
       <c r="AA15" t="n">
-        <v>628604.0</v>
+        <v>628604</v>
       </c>
       <c r="AB15" t="n">
-        <v>134030.0</v>
+        <v>134030</v>
       </c>
       <c r="AC15" t="n">
-        <v>116225.0</v>
+        <v>116225</v>
       </c>
       <c r="AD15" t="n">
-        <v>775627.0</v>
+        <v>775627</v>
       </c>
       <c r="AE15" t="n">
-        <v>173868.0</v>
+        <v>173868</v>
       </c>
       <c r="AF15" t="n">
-        <v>243986.0</v>
+        <v>243986</v>
       </c>
       <c r="AG15" t="n">
-        <v>443313.0</v>
+        <v>443313</v>
       </c>
       <c r="AH15" t="n">
-        <v>187083.0</v>
+        <v>187083</v>
       </c>
       <c r="AI15" t="n">
-        <v>369056.0</v>
+        <v>369056</v>
       </c>
       <c r="AJ15" t="n">
-        <v>108211.0</v>
+        <v>108211</v>
       </c>
       <c r="AK15" t="n">
-        <v>857311.0</v>
+        <v>857311</v>
       </c>
       <c r="AL15" t="n">
-        <v>526387.0</v>
+        <v>526387</v>
       </c>
       <c r="AM15" t="n">
-        <v>142142.0</v>
+        <v>142142</v>
       </c>
       <c r="AN15" t="n">
-        <v>556819.0</v>
+        <v>556819</v>
       </c>
       <c r="AO15" t="n">
-        <v>7844451.0</v>
+        <v>7844451</v>
       </c>
       <c r="AP15" t="n">
-        <v>2757824.0</v>
+        <v>2757824</v>
       </c>
       <c r="AQ15" t="n">
-        <v>1.5054175E7</v>
+        <v>15054175</v>
       </c>
       <c r="AR15" t="n">
-        <v>3355494.0</v>
+        <v>3355494</v>
       </c>
       <c r="AS15" t="n">
-        <v>58524.0</v>
+        <v>58524</v>
       </c>
       <c r="AT15" t="n">
-        <v>62509.0</v>
+        <v>62509</v>
       </c>
       <c r="AU15" t="n">
-        <v>712116.0</v>
+        <v>712116</v>
       </c>
       <c r="AV15" t="n">
-        <v>378206.0</v>
+        <v>378206</v>
       </c>
       <c r="AW15" t="n">
-        <v>4313306.0</v>
+        <v>4313306</v>
       </c>
       <c r="AX15" t="n">
-        <v>170294.0</v>
+        <v>170294</v>
       </c>
       <c r="AY15" t="n">
-        <v>162924.0</v>
+        <v>162924</v>
       </c>
       <c r="AZ15" t="n">
-        <v>200805.0</v>
+        <v>200805</v>
       </c>
       <c r="BA15" t="n">
-        <v>618627.0</v>
+        <v>618627</v>
       </c>
       <c r="BB15" t="n">
-        <v>1081093.0</v>
+        <v>1081093</v>
       </c>
       <c r="BC15" t="n">
-        <v>344380.0</v>
+        <v>344380</v>
       </c>
       <c r="BD15" t="n">
-        <v>1504892.0</v>
+        <v>1504892</v>
       </c>
       <c r="BE15" t="n">
-        <v>529259.0</v>
+        <v>529259</v>
       </c>
       <c r="BF15" t="n">
-        <v>412661.0</v>
+        <v>412661</v>
       </c>
       <c r="BG15" t="n">
-        <v>287433.0</v>
+        <v>287433</v>
       </c>
       <c r="BH15" t="n">
-        <v>3519835.0</v>
+        <v>3519835</v>
       </c>
       <c r="BI15" t="n">
-        <v>718939.0</v>
+        <v>718939</v>
       </c>
       <c r="BJ15" t="n">
-        <v>5158576.0</v>
+        <v>5158576</v>
       </c>
       <c r="BK15" t="n">
-        <v>3803182.0</v>
+        <v>3803182</v>
       </c>
       <c r="BL15" t="n">
-        <v>1815902.0</v>
+        <v>1815902</v>
       </c>
       <c r="BM15" t="n">
-        <v>1562737.0</v>
+        <v>1562737</v>
       </c>
       <c r="BN15" t="n">
-        <v>2198528.0</v>
+        <v>2198528</v>
       </c>
       <c r="BO15" t="n">
-        <v>926849.0</v>
+        <v>926849</v>
       </c>
       <c r="BP15" t="n">
-        <v>3730870.0</v>
+        <v>3730870</v>
       </c>
       <c r="BQ15" t="n">
-        <v>6780014.0</v>
+        <v>6780014</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>